<commit_message>
Implement initial authentication flow and main app for Agente Smith; update .gitignore and remove old CSV files
</commit_message>
<xml_diff>
--- a/output/reporte_consolidado_2025_S27.xlsx
+++ b/output/reporte_consolidado_2025_S27.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,58 +479,58 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P002</t>
+          <t>P001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Galletas Artesanales</t>
+          <t>Cafe Premium</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="E2" t="n">
-        <v>7500</v>
+        <v>26000</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ventas_cali.csv</t>
+          <t>ventas_medellin.csv</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>900000</v>
+        <v>1040000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-10-27</t>
+          <t>2023-10-26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P001</t>
+          <t>P003</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Cafe Premium</t>
+          <t>Chocolatinas</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="E3" t="n">
-        <v>25500</v>
+        <v>2000</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ventas_cali.csv</t>
+          <t>ventas_medellin.csv</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>637500</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="4">
@@ -541,212 +541,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P002</t>
+          <t>P003</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Galletas Artesanales</t>
+          <t>Chocolatinas</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E4" t="n">
-        <v>7600</v>
+        <v>2100</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ventas_cali.csv</t>
+          <t>ventas_medellin.csv</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>608000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2023-10-26</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>P001</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Cafe Premium</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>50</v>
-      </c>
-      <c r="E5" t="n">
-        <v>25000</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ventas_bogota.csv</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1250000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2023-10-26</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>P002</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Galletas Artesanales</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>100</v>
-      </c>
-      <c r="E6" t="n">
-        <v>8000</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ventas_bogota.csv</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2023-10-27</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>P001</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Cafe Premium</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>30</v>
-      </c>
-      <c r="E7" t="n">
-        <v>25000</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>ventas_bogota.csv</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>750000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2023-10-26</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>P001</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Cafe Premium</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>40</v>
-      </c>
-      <c r="E8" t="n">
-        <v>26000</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>ventas_medellin.csv</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1040000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2023-10-26</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>P003</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Chocolatinas</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>200</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>ventas_medellin.csv</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2023-10-27</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>P003</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Chocolatinas</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>150</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2100</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>ventas_medellin.csv</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
         <v>315000</v>
       </c>
     </row>
@@ -761,7 +575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -803,45 +617,27 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="D2" t="n">
-        <v>3677500</v>
+        <v>1040000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P002</t>
+          <t>P003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Galletas Artesanales</t>
+          <t>Chocolatinas</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D3" t="n">
-        <v>2308000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>P003</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Chocolatinas</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>350</v>
-      </c>
-      <c r="D4" t="n">
         <v>715000</v>
       </c>
     </row>

</xml_diff>